<commit_message>
Minor updates to the slides
</commit_message>
<xml_diff>
--- a/raw-data.xlsx
+++ b/raw-data.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">index</t>
+  </si>
   <si>
     <t xml:space="preserve">Sepal.Length</t>
   </si>
@@ -58,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,35 +146,38 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,7 +197,7 @@
         <v>0.2</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,7 +217,7 @@
         <v>0.2</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,7 +237,7 @@
         <v>0.2</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,7 +257,7 @@
         <v>0.2</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +277,7 @@
         <v>0.2</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,7 +297,7 @@
         <v>0.4</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -310,7 +317,7 @@
         <v>0.3</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,7 +337,7 @@
         <v>0.2</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -350,7 +357,7 @@
         <v>0.2</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,7 +377,7 @@
         <v>0.1</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -390,7 +397,7 @@
         <v>0.2</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,7 +417,7 @@
         <v>0.2</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,7 +437,7 @@
         <v>0.1</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,7 +457,7 @@
         <v>0.1</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,7 +477,7 @@
         <v>0.2</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,7 +497,7 @@
         <v>0.4</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +517,7 @@
         <v>0.4</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,7 +537,7 @@
         <v>0.3</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +557,7 @@
         <v>0.3</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,7 +577,7 @@
         <v>0.3</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +597,7 @@
         <v>0.2</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,7 +617,7 @@
         <v>0.4</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,7 +637,7 @@
         <v>0.2</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,7 +657,7 @@
         <v>0.5</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +677,7 @@
         <v>0.2</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,7 +697,7 @@
         <v>0.2</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,7 +717,7 @@
         <v>0.4</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,7 +737,7 @@
         <v>0.2</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,7 +757,7 @@
         <v>0.2</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,7 +777,7 @@
         <v>0.2</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,7 +797,7 @@
         <v>0.2</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +817,7 @@
         <v>0.4</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +837,7 @@
         <v>0.1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +857,7 @@
         <v>0.2</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,7 +877,7 @@
         <v>0.2</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,7 +897,7 @@
         <v>0.2</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +917,7 @@
         <v>0.2</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,7 +937,7 @@
         <v>0.1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +957,7 @@
         <v>0.2</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,7 +977,7 @@
         <v>0.2</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,7 +997,7 @@
         <v>0.3</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1017,7 @@
         <v>0.3</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,7 +1037,7 @@
         <v>0.2</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,7 +1057,7 @@
         <v>0.6</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,7 +1077,7 @@
         <v>0.4</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1097,7 @@
         <v>0.3</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,7 +1117,7 @@
         <v>0.2</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,7 +1137,7 @@
         <v>0.2</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1157,7 @@
         <v>0.2</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,7 +1177,7 @@
         <v>0.2</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,7 +1197,7 @@
         <v>1.4</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,7 +1217,7 @@
         <v>1.5</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1237,7 @@
         <v>1.5</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,7 +1257,7 @@
         <v>1.3</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,7 +1277,7 @@
         <v>1.5</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,7 +1297,7 @@
         <v>1.3</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,7 +1317,7 @@
         <v>1.6</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1357,7 @@
         <v>1.3</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,7 +1377,7 @@
         <v>1.4</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,7 +1417,7 @@
         <v>1.5</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,7 +1457,7 @@
         <v>1.4</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,7 +1477,7 @@
         <v>1.3</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,7 +1497,7 @@
         <v>1.4</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,7 +1517,7 @@
         <v>1.5</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,7 +1557,7 @@
         <v>1.5</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,7 +1577,7 @@
         <v>1.1</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,7 +1597,7 @@
         <v>1.8</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1617,7 @@
         <v>1.3</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1637,7 @@
         <v>1.5</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1657,7 @@
         <v>1.2</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,7 +1677,7 @@
         <v>1.3</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,7 +1697,7 @@
         <v>1.4</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,7 +1717,7 @@
         <v>1.4</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,7 +1737,7 @@
         <v>1.7</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1757,7 @@
         <v>1.5</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1797,7 @@
         <v>1.1</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,7 +1837,7 @@
         <v>1.2</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,7 +1857,7 @@
         <v>1.6</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1877,7 @@
         <v>1.5</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1897,7 @@
         <v>1.6</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,7 +1917,7 @@
         <v>1.5</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +1937,7 @@
         <v>1.3</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,7 +1957,7 @@
         <v>1.3</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,7 +1977,7 @@
         <v>1.3</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,7 +1997,7 @@
         <v>1.2</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,7 +2017,7 @@
         <v>1.4</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,7 +2037,7 @@
         <v>1.2</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,7 +2077,7 @@
         <v>1.3</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2097,7 @@
         <v>1.2</v>
       </c>
       <c r="F97" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,7 +2117,7 @@
         <v>1.3</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2137,7 @@
         <v>1.3</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,7 +2157,7 @@
         <v>1.1</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,7 +2177,7 @@
         <v>1.3</v>
       </c>
       <c r="F101" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2190,7 +2197,7 @@
         <v>2.5</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,7 +2217,7 @@
         <v>1.9</v>
       </c>
       <c r="F103" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,7 +2237,7 @@
         <v>2.1</v>
       </c>
       <c r="F104" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,7 +2257,7 @@
         <v>1.8</v>
       </c>
       <c r="F105" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,7 +2277,7 @@
         <v>2.2</v>
       </c>
       <c r="F106" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2290,7 +2297,7 @@
         <v>2.1</v>
       </c>
       <c r="F107" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2310,7 +2317,7 @@
         <v>1.7</v>
       </c>
       <c r="F108" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2337,7 @@
         <v>1.8</v>
       </c>
       <c r="F109" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2357,7 @@
         <v>1.8</v>
       </c>
       <c r="F110" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,7 +2377,7 @@
         <v>2.5</v>
       </c>
       <c r="F111" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,7 +2397,7 @@
         <v>2</v>
       </c>
       <c r="F112" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2417,7 @@
         <v>1.9</v>
       </c>
       <c r="F113" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2437,7 @@
         <v>2.1</v>
       </c>
       <c r="F114" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="F115" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2470,7 +2477,7 @@
         <v>2.4</v>
       </c>
       <c r="F116" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,7 +2497,7 @@
         <v>2.3</v>
       </c>
       <c r="F117" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,7 +2517,7 @@
         <v>1.8</v>
       </c>
       <c r="F118" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,7 +2537,7 @@
         <v>2.2</v>
       </c>
       <c r="F119" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2557,7 @@
         <v>2.3</v>
       </c>
       <c r="F120" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2577,7 @@
         <v>1.5</v>
       </c>
       <c r="F121" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,7 +2597,7 @@
         <v>2.3</v>
       </c>
       <c r="F122" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2617,7 @@
         <v>2</v>
       </c>
       <c r="F123" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2637,7 @@
         <v>2</v>
       </c>
       <c r="F124" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,7 +2657,7 @@
         <v>1.8</v>
       </c>
       <c r="F125" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2670,7 +2677,7 @@
         <v>2.1</v>
       </c>
       <c r="F126" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,7 +2697,7 @@
         <v>1.8</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,7 +2717,7 @@
         <v>1.8</v>
       </c>
       <c r="F128" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,7 +2737,7 @@
         <v>1.8</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,7 +2757,7 @@
         <v>2.1</v>
       </c>
       <c r="F130" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,7 +2777,7 @@
         <v>1.6</v>
       </c>
       <c r="F131" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2790,7 +2797,7 @@
         <v>1.9</v>
       </c>
       <c r="F132" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2810,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="F133" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2837,7 @@
         <v>2.2</v>
       </c>
       <c r="F134" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2850,7 +2857,7 @@
         <v>1.5</v>
       </c>
       <c r="F135" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2870,7 +2877,7 @@
         <v>1.4</v>
       </c>
       <c r="F136" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2890,7 +2897,7 @@
         <v>2.3</v>
       </c>
       <c r="F137" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2910,7 +2917,7 @@
         <v>2.4</v>
       </c>
       <c r="F138" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,7 +2937,7 @@
         <v>1.8</v>
       </c>
       <c r="F139" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2950,7 +2957,7 @@
         <v>1.8</v>
       </c>
       <c r="F140" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2970,7 +2977,7 @@
         <v>2.1</v>
       </c>
       <c r="F141" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,7 +2997,7 @@
         <v>2.4</v>
       </c>
       <c r="F142" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3010,7 +3017,7 @@
         <v>2.3</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,7 +3037,7 @@
         <v>1.9</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,7 +3057,7 @@
         <v>2.3</v>
       </c>
       <c r="F145" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3070,7 +3077,7 @@
         <v>2.5</v>
       </c>
       <c r="F146" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,7 +3097,7 @@
         <v>2.3</v>
       </c>
       <c r="F147" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,7 +3117,7 @@
         <v>1.9</v>
       </c>
       <c r="F148" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="F149" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,7 +3157,7 @@
         <v>2.3</v>
       </c>
       <c r="F150" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3170,7 +3177,7 @@
         <v>1.8</v>
       </c>
       <c r="F151" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>